<commit_message>
Updated the sample files for bulk upload
</commit_message>
<xml_diff>
--- a/public/sample-distributors.xlsx
+++ b/public/sample-distributors.xlsx
@@ -1,97 +1,85 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kehindeehinmitan/Projects/Orange/depleteiq/client/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kehindeehinmitan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE581806-10EE-164F-958A-B5B55EC369DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C86D8C-4B50-C844-AD31-18F13311D859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>role_id</t>
-  </si>
-  <si>
-    <t>send_notification</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Doe</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>john.doe@example.com</t>
-  </si>
-  <si>
-    <t>jane.smith@example.com</t>
-  </si>
-  <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>0987654321</t>
-  </si>
-  <si>
-    <t>pass123</t>
-  </si>
-  <si>
-    <t>secure456</t>
-  </si>
-  <si>
-    <t>business_name</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>ime_vss_user_id</t>
-  </si>
-  <si>
-    <t>Shola and sons</t>
-  </si>
-  <si>
-    <t>orange &amp; drugs Ltd.</t>
-  </si>
-  <si>
-    <t>Town planning</t>
-  </si>
-  <si>
-    <t>24dd1ea1-a1e3-406c-b58c-305ecc4984bb</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>ImeVssUser</t>
+  </si>
+  <si>
+    <t>BusinessName</t>
+  </si>
+  <si>
+    <t>BusinessAddress</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>emily.clark@example.com</t>
+  </si>
+  <si>
+    <t>5678901234</t>
+  </si>
+  <si>
+    <t>imevss1@example.com</t>
+  </si>
+  <si>
+    <t>Clark Supplies</t>
+  </si>
+  <si>
+    <t>Mushin market</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>david.lee@example.com</t>
+  </si>
+  <si>
+    <t>6789012345</t>
+  </si>
+  <si>
+    <t>imevss2@example.com</t>
+  </si>
+  <si>
+    <t>Lee Distributors</t>
   </si>
 </sst>
 </file>
@@ -103,7 +91,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -111,14 +98,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3D0319"/>
-      <name val="Courier New"/>
-      <family val="1"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,27 +138,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -181,7 +153,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -194,9 +166,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -234,84 +206,24 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -334,7 +246,7 @@
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -425,7 +337,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -447,11 +359,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
+          <a:path path="circle"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -466,9 +376,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:path path="circle"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -480,27 +388,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="21.5" customWidth="1"/>
-    <col min="10" max="10" width="45.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="22.5" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,81 +424,58 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>